<commit_message>
Fix mistakes on project 01
</commit_message>
<xml_diff>
--- a/30days.xlsx
+++ b/30days.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedrohenriqueserafim/Documents/Computer Science/Courses/Nanodegree/Data Structure and Algorithms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedrohenriqueserafim/Documents/Computer Science/Nanodegree/udacity - data structure and algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7AC7D3-4DDF-EC4B-B491-F491767F3B30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFEE0AE-F13F-FE45-8983-F8A88410984F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16460" xr2:uid="{369082CA-E6F1-314F-95E9-EA76C66D6972}"/>
+    <workbookView xWindow="-34700" yWindow="-480" windowWidth="28240" windowHeight="16460" xr2:uid="{369082CA-E6F1-314F-95E9-EA76C66D6972}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Day 1</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>Finishing Python Review: Control Flow, Functions, Scripting and Advanced Topics.</t>
+  </si>
+  <si>
+    <t>Day 7</t>
+  </si>
+  <si>
+    <t>Finish project 01 (Scrumble Computer Science Problems) and start arrays and linked lists.</t>
+  </si>
+  <si>
+    <t>Day 8</t>
+  </si>
+  <si>
+    <t>Day 9</t>
   </si>
 </sst>
 </file>
@@ -413,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825D045E-AC2A-0E46-ABE8-67FC370BCBF0}">
-  <dimension ref="B4:D9"/>
+  <dimension ref="B4:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="69.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
@@ -490,6 +502,27 @@
         <v>44097</v>
       </c>
     </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44098</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Start coding LRU Cache
</commit_message>
<xml_diff>
--- a/30days.xlsx
+++ b/30days.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedrohenriqueserafim/Documents/Computer Science/Nanodegree/udacity - data structure and algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFEE0AE-F13F-FE45-8983-F8A88410984F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415CA2CF-5D11-5C44-BC28-FB5017FBBE03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34700" yWindow="-480" windowWidth="28240" windowHeight="16460" xr2:uid="{369082CA-E6F1-314F-95E9-EA76C66D6972}"/>
+    <workbookView xWindow="500" yWindow="940" windowWidth="28240" windowHeight="16440" xr2:uid="{369082CA-E6F1-314F-95E9-EA76C66D6972}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Day 1</t>
   </si>
@@ -73,6 +73,51 @@
   </si>
   <si>
     <t>Day 9</t>
+  </si>
+  <si>
+    <t>Working with arrays and linked lists.</t>
+  </si>
+  <si>
+    <t>Day 10</t>
+  </si>
+  <si>
+    <t>Day 11</t>
+  </si>
+  <si>
+    <t>Finish lesson about arrays and linked lists.</t>
+  </si>
+  <si>
+    <t>Day 12</t>
+  </si>
+  <si>
+    <t>Finish lesson about stacks and queues.</t>
+  </si>
+  <si>
+    <t>Day 13</t>
+  </si>
+  <si>
+    <t>Day 14</t>
+  </si>
+  <si>
+    <t>Working on the lesson about recursion</t>
+  </si>
+  <si>
+    <t>Working on the lesson about trees</t>
+  </si>
+  <si>
+    <t>Day 15</t>
+  </si>
+  <si>
+    <t>Day 16</t>
+  </si>
+  <si>
+    <t>Day 17</t>
+  </si>
+  <si>
+    <t>Finish lesson about trees</t>
+  </si>
+  <si>
+    <t>Working on the lesson about hashing</t>
   </si>
 </sst>
 </file>
@@ -425,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825D045E-AC2A-0E46-ABE8-67FC370BCBF0}">
-  <dimension ref="B4:D12"/>
+  <dimension ref="B4:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,10 +562,110 @@
       <c r="B11" t="s">
         <v>14</v>
       </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44099</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44101</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44102</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44103</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44104</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44105</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1">
+        <v>44106</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="1">
+        <v>44107</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="1">
+        <v>44108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add red black tree algorithm
</commit_message>
<xml_diff>
--- a/30days.xlsx
+++ b/30days.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedrohenriqueserafim/Documents/Computer Science/Nanodegree/udacity - data structure and algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D91CF77-B790-2748-BB7B-06083698E481}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEFC63A-6C79-2940-92AF-D0AA6F669370}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32440" yWindow="-80" windowWidth="28240" windowHeight="16440" xr2:uid="{369082CA-E6F1-314F-95E9-EA76C66D6972}"/>
+    <workbookView xWindow="-35260" yWindow="580" windowWidth="28240" windowHeight="16440" xr2:uid="{369082CA-E6F1-314F-95E9-EA76C66D6972}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Day 1</t>
   </si>
@@ -162,6 +162,64 @@
   </si>
   <si>
     <t>Day 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Finished project 02 (Show me the Data Structure)
+- Worked on explanations for the project 02 problems</t>
+  </si>
+  <si>
+    <t>Day 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Fix problems on project 02 (Show me the Data Structure)
+- Search for books on the subject</t>
+  </si>
+  <si>
+    <t>Day 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Learning about Binary Search
+- Reading the book "Introduction to Algorithm"</t>
+  </si>
+  <si>
+    <t>Day 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Worked on Tries and Heaps.</t>
+  </si>
+  <si>
+    <t>Day 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Learned about self-balancing trees
+- Studied about Red-Black Trees</t>
+  </si>
+  <si>
+    <t>Day 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Start studying sorting algorithms.
+- I've learned about Bubble Sorted.
+- I've solved some exercises.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - I've learned about Merge Sort.
+- I've solved some exercises.</t>
+  </si>
+  <si>
+    <t>Day 30</t>
+  </si>
+  <si>
+    <t>Day 31</t>
+  </si>
+  <si>
+    <t>Day 32</t>
+  </si>
+  <si>
+    <t>I've learned about Quick Sort</t>
+  </si>
+  <si>
+    <t>I've learned about Heap Sort</t>
   </si>
 </sst>
 </file>
@@ -522,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825D045E-AC2A-0E46-ABE8-67FC370BCBF0}">
-  <dimension ref="B4:D27"/>
+  <dimension ref="B4:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,12 +846,100 @@
         <v>44114</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="C27" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="D27" s="2">
         <v>44115</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="2">
+        <v>44116</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="2">
+        <v>44117</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="2">
+        <v>44118</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="2">
+        <v>44119</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="2">
+        <v>44120</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="2">
+        <v>44121</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="2">
+        <v>44122</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>